<commit_message>
Added EXST1 model; tests only compare data for generator speed, tm and vf;
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_sexs.xlsx
+++ b/andes/cases/kundur/kundur_sexs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05125EC4-B7B0-624F-884E-A35A3FDA479A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C794B35F-5C63-AB4C-99E7-76700E6D3EB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="27860" windowHeight="17580" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,18 +316,6 @@
     <t>TE</t>
   </si>
   <si>
-    <t>EXDC2_1</t>
-  </si>
-  <si>
-    <t>EXDC2_2</t>
-  </si>
-  <si>
-    <t>EXDC2_3</t>
-  </si>
-  <si>
-    <t>EXDC2_4</t>
-  </si>
-  <si>
     <t>model</t>
   </si>
   <si>
@@ -353,6 +341,18 @@
   </si>
   <si>
     <t>EMAX</t>
+  </si>
+  <si>
+    <t>SEXS_1</t>
+  </si>
+  <si>
+    <t>SEXS_2</t>
+  </si>
+  <si>
+    <t>SEXS_3</t>
+  </si>
+  <si>
+    <t>SEXS_4</t>
   </si>
 </sst>
 </file>
@@ -1277,13 +1277,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1297,10 +1297,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F2" t="s">
         <v>51</v>
@@ -3536,7 +3536,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3558,22 +3558,22 @@
         <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>93</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>94</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -3587,7 +3587,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3622,7 +3622,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -3657,7 +3657,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -3692,7 +3692,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="E5">
         <v>4</v>

</xml_diff>